<commit_message>
first attemp at containerization - replace 127.0.0.1 with localhost in js file
</commit_message>
<xml_diff>
--- a/app/football_statistics_2025_26.xlsx
+++ b/app/football_statistics_2025_26.xlsx
@@ -437,11 +437,11 @@
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="19" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
     <col width="17" customWidth="1" min="6" max="6"/>
-    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
     <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="11" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
     <col width="26" customWidth="1" min="10" max="10"/>
     <col width="24" customWidth="1" min="11" max="11"/>
     <col width="15" customWidth="1" min="12" max="12"/>
@@ -454,7 +454,7 @@
     <col width="17" customWidth="1" min="19" max="19"/>
     <col width="12" customWidth="1" min="20" max="20"/>
     <col width="19" customWidth="1" min="21" max="21"/>
-    <col width="11" customWidth="1" min="22" max="22"/>
+    <col width="12" customWidth="1" min="22" max="22"/>
     <col width="27" customWidth="1" min="23" max="23"/>
     <col width="25" customWidth="1" min="24" max="24"/>
     <col width="15" customWidth="1" min="25" max="25"/>
@@ -463,11 +463,11 @@
     <col width="27" customWidth="1" min="28" max="28"/>
     <col width="20" customWidth="1" min="29" max="29"/>
     <col width="17" customWidth="1" min="30" max="30"/>
-    <col width="12" customWidth="1" min="31" max="31"/>
+    <col width="11" customWidth="1" min="31" max="31"/>
     <col width="18" customWidth="1" min="32" max="32"/>
-    <col width="12" customWidth="1" min="33" max="33"/>
+    <col width="11" customWidth="1" min="33" max="33"/>
     <col width="19" customWidth="1" min="34" max="34"/>
-    <col width="12" customWidth="1" min="35" max="35"/>
+    <col width="11" customWidth="1" min="35" max="35"/>
     <col width="27" customWidth="1" min="36" max="36"/>
     <col width="25" customWidth="1" min="37" max="37"/>
     <col width="15" customWidth="1" min="38" max="38"/>
@@ -695,19 +695,19 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>100</v>
+        <v>66.67</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0</v>
+        <v>33.33</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0</v>
@@ -716,22 +716,22 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>3</v>
+        <v>2.33</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" s="1" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="O2" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="P2" s="1" t="n">
         <v>2</v>
@@ -773,43 +773,43 @@
         <v>0</v>
       </c>
       <c r="AC2" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AD2" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE2" s="1" t="n">
-        <v>66.67</v>
+        <v>60</v>
       </c>
       <c r="AF2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG2" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AH2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AI2" s="1" t="n">
-        <v>33.33</v>
+        <v>20</v>
       </c>
       <c r="AJ2" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AK2" s="1" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AL2" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AM2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN2" s="1" t="n">
-        <v>0.33</v>
+        <v>0.4</v>
       </c>
       <c r="AO2" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -863,82 +863,82 @@
         <v>2</v>
       </c>
       <c r="P3" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R3" s="1" t="n">
-        <v>100</v>
+        <v>33.33</v>
       </c>
       <c r="S3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" s="1" t="n">
-        <v>0</v>
+        <v>33.33</v>
       </c>
       <c r="U3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3" s="1" t="n">
-        <v>0</v>
+        <v>33.33</v>
       </c>
       <c r="W3" s="1" t="n">
-        <v>3</v>
+        <v>1.33</v>
       </c>
       <c r="X3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="Z3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="Y3" s="1" t="n">
+      <c r="AA3" s="1" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="AB3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="Z3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AC3" s="1" t="n">
-        <v>3</v>
-      </c>
       <c r="AD3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AE3" s="1" t="n">
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AF3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG3" s="1" t="n">
-        <v>33.33</v>
+        <v>40</v>
       </c>
       <c r="AH3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI3" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AJ3" s="1" t="n">
-        <v>2.33</v>
+        <v>1.6</v>
       </c>
       <c r="AK3" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AL3" s="1" t="n">
-        <v>2.33</v>
+        <v>2</v>
       </c>
       <c r="AM3" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AN3" s="1" t="n">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="AO3" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -953,10 +953,10 @@
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>100</v>
@@ -977,25 +977,25 @@
         <v>3</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>2.5</v>
+        <v>2.33</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P4" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>100</v>
@@ -1016,25 +1016,25 @@
         <v>3</v>
       </c>
       <c r="X4" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y4" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Z4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AA4" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB4" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC4" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AD4" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AE4" s="1" t="n">
         <v>100</v>
@@ -1055,19 +1055,19 @@
         <v>3</v>
       </c>
       <c r="AK4" s="1" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="AL4" s="1" t="n">
-        <v>2.67</v>
+        <v>2.2</v>
       </c>
       <c r="AM4" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AN4" s="1" t="n">
-        <v>1.33</v>
+        <v>1</v>
       </c>
       <c r="AO4" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -1082,13 +1082,13 @@
         </is>
       </c>
       <c r="C5" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>0</v>
@@ -1100,103 +1100,103 @@
         <v>1</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="M5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="N5" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O5" s="1" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="P5" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R5" s="1" t="n">
-        <v>50</v>
+        <v>33.33</v>
       </c>
       <c r="S5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" s="1" t="n">
-        <v>0</v>
+        <v>33.33</v>
       </c>
       <c r="U5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="V5" s="1" t="n">
-        <v>50</v>
+        <v>33.33</v>
       </c>
       <c r="W5" s="1" t="n">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
       <c r="X5" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="Y5" s="1" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="Z5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC5" s="1" t="n">
-        <v>3</v>
-      </c>
       <c r="AD5" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE5" s="1" t="n">
-        <v>33.33</v>
+        <v>40</v>
       </c>
       <c r="AF5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG5" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AH5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AI5" s="1" t="n">
-        <v>66.67</v>
+        <v>40</v>
       </c>
       <c r="AJ5" s="1" t="n">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="AK5" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="AL5" s="1" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AM5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AL5" s="1" t="n">
-        <v>1.67</v>
-      </c>
-      <c r="AM5" s="1" t="n">
-        <v>4</v>
-      </c>
       <c r="AN5" s="1" t="n">
-        <v>1.33</v>
+        <v>1</v>
       </c>
       <c r="AO5" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -1211,121 +1211,121 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1" t="n">
+      <c r="U6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V6" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="J6" s="1" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="L6" s="1" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="M6" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="N6" s="1" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="O6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="T6" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="U6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V6" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="W6" s="1" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="X6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="Y6" s="1" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Z6" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AA6" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB6" s="1" t="n">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AC6" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AD6" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE6" s="1" t="n">
-        <v>33.33</v>
+        <v>40</v>
       </c>
       <c r="AF6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AG6" s="1" t="n">
-        <v>33.33</v>
+        <v>20</v>
       </c>
       <c r="AH6" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI6" s="1" t="n">
-        <v>33.33</v>
+        <v>40</v>
       </c>
       <c r="AJ6" s="1" t="n">
-        <v>1.33</v>
+        <v>1.4</v>
       </c>
       <c r="AK6" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AL6" s="1" t="n">
-        <v>1.33</v>
+        <v>1.2</v>
       </c>
       <c r="AM6" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AN6" s="1" t="n">
-        <v>1.33</v>
+        <v>1.6</v>
       </c>
       <c r="AO6" s="1" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="7">
@@ -1430,19 +1430,19 @@
         </is>
       </c>
       <c r="C9" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>0</v>
@@ -1451,25 +1451,25 @@
         <v>0</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="M9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="N9" s="1" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O9" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P9" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q9" s="1" t="n">
         <v>0</v>
@@ -1478,73 +1478,73 @@
         <v>0</v>
       </c>
       <c r="S9" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T9" s="1" t="n">
-        <v>50</v>
+        <v>66.67</v>
       </c>
       <c r="U9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>50</v>
+        <v>33.33</v>
       </c>
       <c r="W9" s="1" t="n">
-        <v>0.5</v>
+        <v>0.67</v>
       </c>
       <c r="X9" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="Z9" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA9" s="1" t="n">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
       <c r="AB9" s="1" t="n">
         <v>-1</v>
       </c>
       <c r="AC9" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AD9" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE9" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AF9" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG9" s="1" t="n">
-        <v>66.67</v>
+        <v>60</v>
       </c>
       <c r="AH9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AI9" s="1" t="n">
-        <v>33.33</v>
+        <v>20</v>
       </c>
       <c r="AJ9" s="1" t="n">
-        <v>0.67</v>
+        <v>1.2</v>
       </c>
       <c r="AK9" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AL9" s="1" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="AM9" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AN9" s="1" t="n">
-        <v>1.33</v>
+        <v>1</v>
       </c>
       <c r="AO9" s="1" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1559,13 +1559,13 @@
         </is>
       </c>
       <c r="C10" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>0</v>
@@ -1580,13 +1580,13 @@
         <v>0</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="M10" s="1" t="n">
         <v>0</v>
@@ -1595,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="1" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="P10" s="1" t="n">
         <v>3</v>
@@ -1637,19 +1637,19 @@
         <v>4</v>
       </c>
       <c r="AC10" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AD10" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE10" s="1" t="n">
-        <v>66.67</v>
+        <v>80</v>
       </c>
       <c r="AF10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AG10" s="1" t="n">
-        <v>33.33</v>
+        <v>20</v>
       </c>
       <c r="AH10" s="1" t="n">
         <v>0</v>
@@ -1658,22 +1658,22 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="1" t="n">
-        <v>2.33</v>
+        <v>2.6</v>
       </c>
       <c r="AK10" s="1" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AL10" s="1" t="n">
-        <v>2.33</v>
+        <v>3.2</v>
       </c>
       <c r="AM10" s="1" t="n">
         <v>3</v>
       </c>
       <c r="AN10" s="1" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="AO10" s="1" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -1688,10 +1688,10 @@
         </is>
       </c>
       <c r="C11" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>100</v>
@@ -1712,25 +1712,25 @@
         <v>3</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>1.5</v>
+        <v>1.67</v>
       </c>
       <c r="M11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>0.5</v>
+        <v>0.33</v>
       </c>
       <c r="O11" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" s="1" t="n">
         <v>100</v>
@@ -1751,25 +1751,25 @@
         <v>3</v>
       </c>
       <c r="X11" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y11" s="1" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="Z11" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA11" s="1" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AB11" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC11" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AD11" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AE11" s="1" t="n">
         <v>100</v>
@@ -1790,19 +1790,19 @@
         <v>3</v>
       </c>
       <c r="AK11" s="1" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AL11" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AM11" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN11" s="1" t="n">
-        <v>0.33</v>
+        <v>0.4</v>
       </c>
       <c r="AO11" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
@@ -1907,43 +1907,43 @@
         </is>
       </c>
       <c r="C14" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>0</v>
+        <v>33.33</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0</v>
+        <v>33.33</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>100</v>
+        <v>33.33</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>0</v>
+        <v>1.33</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L14" s="1" t="n">
-        <v>1</v>
+        <v>1.67</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N14" s="1" t="n">
-        <v>2</v>
+        <v>1.33</v>
       </c>
       <c r="O14" s="1" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="P14" s="1" t="n">
         <v>1</v>
@@ -1985,16 +1985,16 @@
         <v>0</v>
       </c>
       <c r="AC14" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD14" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE14" s="1" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AF14" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG14" s="1" t="n">
         <v>50</v>
@@ -2003,25 +2003,25 @@
         <v>1</v>
       </c>
       <c r="AI14" s="1" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="AJ14" s="1" t="n">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="AK14" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AL14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AM14" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AN14" s="1" t="n">
-        <v>2.5</v>
+        <v>1.75</v>
       </c>
       <c r="AO14" s="1" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -2036,10 +2036,10 @@
         </is>
       </c>
       <c r="C15" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>100</v>
@@ -2060,10 +2060,10 @@
         <v>3</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="L15" s="1" t="n">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="M15" s="1" t="n">
         <v>0</v>
@@ -2072,13 +2072,13 @@
         <v>0</v>
       </c>
       <c r="O15" s="1" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R15" s="1" t="n">
         <v>100</v>
@@ -2099,25 +2099,25 @@
         <v>3</v>
       </c>
       <c r="X15" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Y15" s="1" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="Z15" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA15" s="1" t="n">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB15" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AC15" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD15" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE15" s="1" t="n">
         <v>100</v>
@@ -2138,19 +2138,19 @@
         <v>3</v>
       </c>
       <c r="AK15" s="1" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="AL15" s="1" t="n">
         <v>4.5</v>
       </c>
       <c r="AM15" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AN15" s="1" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AO15" s="1" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
@@ -2165,10 +2165,10 @@
         </is>
       </c>
       <c r="C16" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>100</v>
@@ -2189,10 +2189,10 @@
         <v>3</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L16" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M16" s="1" t="n">
         <v>0</v>
@@ -2201,22 +2201,22 @@
         <v>0</v>
       </c>
       <c r="O16" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P16" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q16" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="S16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T16" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="U16" s="1" t="n">
         <v>0</v>
@@ -2225,37 +2225,37 @@
         <v>0</v>
       </c>
       <c r="W16" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X16" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y16" s="1" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="Z16" s="1" t="n">
         <v>3</v>
       </c>
       <c r="AA16" s="1" t="n">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="AB16" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC16" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD16" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AE16" s="1" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="AF16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AG16" s="1" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="AH16" s="1" t="n">
         <v>0</v>
@@ -2264,22 +2264,22 @@
         <v>0</v>
       </c>
       <c r="AJ16" s="1" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AK16" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="AL16" s="1" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="AM16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN16" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AO16" s="1" t="n">
         <v>6</v>
-      </c>
-      <c r="AL16" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM16" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN16" s="1" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="AO16" s="1" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -2294,13 +2294,13 @@
         </is>
       </c>
       <c r="C17" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>0</v>
@@ -2309,37 +2309,37 @@
         <v>0</v>
       </c>
       <c r="H17" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="J17" s="1" t="n">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L17" s="1" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="M17" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="O17" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P17" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R17" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="S17" s="1" t="n">
         <v>0</v>
@@ -2348,37 +2348,37 @@
         <v>0</v>
       </c>
       <c r="U17" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V17" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="W17" s="1" t="n">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="X17" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y17" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Z17" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AA17" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB17" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC17" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD17" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AE17" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="AF17" s="1" t="n">
         <v>0</v>
@@ -2387,28 +2387,28 @@
         <v>0</v>
       </c>
       <c r="AH17" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI17" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AJ17" s="1" t="n">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="AK17" s="1" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AL17" s="1" t="n">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="AM17" s="1" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="AN17" s="1" t="n">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="AO17" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -2423,7 +2423,7 @@
         </is>
       </c>
       <c r="C18" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>0</v>
@@ -2438,7 +2438,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
         <v>100</v>
@@ -2453,28 +2453,28 @@
         <v>0</v>
       </c>
       <c r="M18" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="O18" s="1" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="P18" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R18" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="S18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T18" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="U18" s="1" t="n">
         <v>0</v>
@@ -2483,61 +2483,61 @@
         <v>0</v>
       </c>
       <c r="W18" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X18" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Y18" s="1" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="Z18" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AB18" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC18" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD18" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE18" s="1" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AF18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AG18" s="1" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="AH18" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI18" s="1" t="n">
         <v>50</v>
       </c>
       <c r="AJ18" s="1" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AK18" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AL18" s="1" t="n">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="AM18" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AN18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AO18" s="1" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -2552,10 +2552,10 @@
         </is>
       </c>
       <c r="C19" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>100</v>
@@ -2576,28 +2576,28 @@
         <v>3</v>
       </c>
       <c r="K19" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L19" s="1" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="M19" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O19" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P19" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="S19" s="1" t="n">
         <v>0</v>
@@ -2609,64 +2609,64 @@
         <v>1</v>
       </c>
       <c r="V19" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="W19" s="1" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="X19" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y19" s="1" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Z19" s="1" t="n">
         <v>6</v>
       </c>
       <c r="AA19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB19" s="1" t="n">
+        <v>-5</v>
+      </c>
+      <c r="AC19" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE19" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="AF19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI19" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ19" s="1" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="AK19" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="AB19" s="1" t="n">
-        <v>-6</v>
-      </c>
-      <c r="AC19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE19" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="AF19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI19" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="AJ19" s="1" t="n">
+      <c r="AL19" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="AK19" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL19" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="AM19" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AN19" s="1" t="n">
-        <v>3</v>
+        <v>1.75</v>
       </c>
       <c r="AO19" s="1" t="n">
-        <v>-4</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="20">
@@ -2681,10 +2681,10 @@
         </is>
       </c>
       <c r="C20" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>100</v>
@@ -2705,10 +2705,10 @@
         <v>3</v>
       </c>
       <c r="K20" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L20" s="1" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="M20" s="1" t="n">
         <v>0</v>
@@ -2717,10 +2717,10 @@
         <v>0</v>
       </c>
       <c r="O20" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P20" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q20" s="1" t="n">
         <v>0</v>
@@ -2735,7 +2735,7 @@
         <v>0</v>
       </c>
       <c r="U20" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V20" s="1" t="n">
         <v>100</v>
@@ -2744,25 +2744,25 @@
         <v>0</v>
       </c>
       <c r="X20" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="Z20" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AA20" s="1" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB20" s="1" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AC20" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD20" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE20" s="1" t="n">
         <v>50</v>
@@ -2774,7 +2774,7 @@
         <v>0</v>
       </c>
       <c r="AH20" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI20" s="1" t="n">
         <v>50</v>
@@ -2783,16 +2783,16 @@
         <v>1.5</v>
       </c>
       <c r="AK20" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AL20" s="1" t="n">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="AM20" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AN20" s="1" t="n">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="AO20" s="1" t="n">
         <v>0</v>
@@ -2900,13 +2900,13 @@
         </is>
       </c>
       <c r="C23" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>0</v>
@@ -2918,13 +2918,13 @@
         <v>1</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J23" s="1" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K23" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L23" s="1" t="n">
         <v>1</v>
@@ -2933,16 +2933,16 @@
         <v>2</v>
       </c>
       <c r="N23" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O23" s="1" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P23" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R23" s="1" t="n">
         <v>100</v>
@@ -2963,10 +2963,10 @@
         <v>3</v>
       </c>
       <c r="X23" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Y23" s="1" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="Z23" s="1" t="n">
         <v>0</v>
@@ -2975,16 +2975,16 @@
         <v>0</v>
       </c>
       <c r="AB23" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AC23" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD23" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AE23" s="1" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="AF23" s="1" t="n">
         <v>0</v>
@@ -2996,25 +2996,25 @@
         <v>1</v>
       </c>
       <c r="AI23" s="1" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="AJ23" s="1" t="n">
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
       <c r="AK23" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AL23" s="1" t="n">
-        <v>1.5</v>
+        <v>1.75</v>
       </c>
       <c r="AM23" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AN23" s="1" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AO23" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
@@ -3029,13 +3029,13 @@
         </is>
       </c>
       <c r="C24" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>50</v>
+        <v>66.67</v>
       </c>
       <c r="F24" s="1" t="n">
         <v>0</v>
@@ -3047,28 +3047,28 @@
         <v>1</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>50</v>
+        <v>33.33</v>
       </c>
       <c r="J24" s="1" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="K24" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L24" s="1" t="n">
-        <v>3</v>
+        <v>2.67</v>
       </c>
       <c r="M24" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N24" s="1" t="n">
         <v>1</v>
       </c>
       <c r="O24" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P24" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="1" t="n">
         <v>0</v>
@@ -3083,34 +3083,34 @@
         <v>0</v>
       </c>
       <c r="U24" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V24" s="1" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W24" s="1" t="n">
         <v>0</v>
       </c>
       <c r="X24" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y24" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z24" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA24" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB24" s="1" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC24" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD24" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE24" s="1" t="n">
         <v>50</v>
@@ -3122,7 +3122,7 @@
         <v>0</v>
       </c>
       <c r="AH24" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI24" s="1" t="n">
         <v>50</v>
@@ -3131,16 +3131,16 @@
         <v>1.5</v>
       </c>
       <c r="AK24" s="1" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="AL24" s="1" t="n">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="AM24" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AN24" s="1" t="n">
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="AO24" s="1" t="n">
         <v>4</v>
@@ -3158,10 +3158,10 @@
         </is>
       </c>
       <c r="C25" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="1" t="n">
         <v>100</v>
@@ -3182,34 +3182,34 @@
         <v>3</v>
       </c>
       <c r="K25" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L25" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M25" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N25" s="1" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="O25" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P25" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q25" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R25" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="S25" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="U25" s="1" t="n">
         <v>0</v>
@@ -3218,37 +3218,37 @@
         <v>0</v>
       </c>
       <c r="W25" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X25" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y25" s="1" t="n">
         <v>1</v>
       </c>
       <c r="Z25" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA25" s="1" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AB25" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AC25" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD25" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE25" s="1" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="AF25" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG25" s="1" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AH25" s="1" t="n">
         <v>0</v>
@@ -3257,22 +3257,22 @@
         <v>0</v>
       </c>
       <c r="AJ25" s="1" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AK25" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AL25" s="1" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AM25" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN25" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO25" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
@@ -3287,13 +3287,13 @@
         </is>
       </c>
       <c r="C26" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F26" s="1" t="n">
         <v>0</v>
@@ -3302,31 +3302,31 @@
         <v>0</v>
       </c>
       <c r="H26" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="J26" s="1" t="n">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="K26" s="1" t="n">
         <v>4</v>
       </c>
       <c r="L26" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M26" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O26" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P26" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q26" s="1" t="n">
         <v>0</v>
@@ -3341,7 +3341,7 @@
         <v>0</v>
       </c>
       <c r="U26" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V26" s="1" t="n">
         <v>100</v>
@@ -3356,22 +3356,22 @@
         <v>0</v>
       </c>
       <c r="Z26" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA26" s="1" t="n">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB26" s="1" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AC26" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD26" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AE26" s="1" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="AF26" s="1" t="n">
         <v>0</v>
@@ -3380,28 +3380,28 @@
         <v>0</v>
       </c>
       <c r="AH26" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AI26" s="1" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="AJ26" s="1" t="n">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="AK26" s="1" t="n">
         <v>4</v>
       </c>
       <c r="AL26" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AM26" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AN26" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AO26" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -3455,10 +3455,10 @@
         <v>1</v>
       </c>
       <c r="P27" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q27" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R27" s="1" t="n">
         <v>100</v>
@@ -3479,25 +3479,25 @@
         <v>3</v>
       </c>
       <c r="X27" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Y27" s="1" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="Z27" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA27" s="1" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AB27" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AC27" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD27" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE27" s="1" t="n">
         <v>100</v>
@@ -3518,19 +3518,19 @@
         <v>3</v>
       </c>
       <c r="AK27" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AL27" s="1" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AM27" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN27" s="1" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="AO27" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
@@ -3545,13 +3545,13 @@
         </is>
       </c>
       <c r="C28" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F28" s="1" t="n">
         <v>0</v>
@@ -3560,34 +3560,34 @@
         <v>0</v>
       </c>
       <c r="H28" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="J28" s="1" t="n">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="K28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L28" s="1" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M28" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28" s="1" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O28" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P28" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q28" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R28" s="1" t="n">
         <v>100</v>
@@ -3608,7 +3608,7 @@
         <v>3</v>
       </c>
       <c r="X28" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y28" s="1" t="n">
         <v>1</v>
@@ -3620,16 +3620,16 @@
         <v>0</v>
       </c>
       <c r="AB28" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC28" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD28" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE28" s="1" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="AF28" s="1" t="n">
         <v>0</v>
@@ -3638,25 +3638,25 @@
         <v>0</v>
       </c>
       <c r="AH28" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI28" s="1" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AJ28" s="1" t="n">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="AK28" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL28" s="1" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AM28" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN28" s="1" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AO28" s="1" t="n">
         <v>2</v>
@@ -3764,10 +3764,10 @@
         </is>
       </c>
       <c r="C31" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" s="1" t="n">
         <v>100</v>
@@ -3788,97 +3788,97 @@
         <v>3</v>
       </c>
       <c r="K31" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L31" s="1" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="M31" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N31" s="1" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O31" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P31" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R31" s="1" t="n">
-        <v>50</v>
+        <v>33.33</v>
       </c>
       <c r="S31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T31" s="1" t="n">
-        <v>50</v>
+        <v>33.33</v>
       </c>
       <c r="U31" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V31" s="1" t="n">
-        <v>0</v>
+        <v>33.33</v>
       </c>
       <c r="W31" s="1" t="n">
-        <v>2</v>
+        <v>1.33</v>
       </c>
       <c r="X31" s="1" t="n">
         <v>10</v>
       </c>
       <c r="Y31" s="1" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="Z31" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA31" s="1" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="AB31" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC31" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="Z31" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB31" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="AC31" s="1" t="n">
-        <v>3</v>
-      </c>
       <c r="AD31" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE31" s="1" t="n">
-        <v>66.67</v>
+        <v>60</v>
       </c>
       <c r="AF31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AG31" s="1" t="n">
-        <v>33.33</v>
+        <v>20</v>
       </c>
       <c r="AH31" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI31" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AJ31" s="1" t="n">
-        <v>2.33</v>
+        <v>2</v>
       </c>
       <c r="AK31" s="1" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AL31" s="1" t="n">
-        <v>3.67</v>
+        <v>2.6</v>
       </c>
       <c r="AM31" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AN31" s="1" t="n">
-        <v>1.33</v>
+        <v>1.6</v>
       </c>
       <c r="AO31" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
@@ -3893,10 +3893,10 @@
         </is>
       </c>
       <c r="C32" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E32" s="1" t="n">
         <v>100</v>
@@ -3917,10 +3917,10 @@
         <v>3</v>
       </c>
       <c r="K32" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L32" s="1" t="n">
-        <v>2</v>
+        <v>1.67</v>
       </c>
       <c r="M32" s="1" t="n">
         <v>0</v>
@@ -3929,16 +3929,16 @@
         <v>0</v>
       </c>
       <c r="O32" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P32" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R32" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="S32" s="1" t="n">
         <v>0</v>
@@ -3947,37 +3947,37 @@
         <v>0</v>
       </c>
       <c r="U32" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V32" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="W32" s="1" t="n">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="X32" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="Z32" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA32" s="1" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AB32" s="1" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC32" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AD32" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE32" s="1" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="AF32" s="1" t="n">
         <v>0</v>
@@ -3986,28 +3986,28 @@
         <v>0</v>
       </c>
       <c r="AH32" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI32" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AJ32" s="1" t="n">
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="AK32" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AL32" s="1" t="n">
-        <v>1.67</v>
+        <v>1.4</v>
       </c>
       <c r="AM32" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN32" s="1" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AO32" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
@@ -4022,10 +4022,10 @@
         </is>
       </c>
       <c r="C33" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="1" t="n">
         <v>100</v>
@@ -4046,19 +4046,19 @@
         <v>3</v>
       </c>
       <c r="K33" s="1" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L33" s="1" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="M33" s="1" t="n">
         <v>2</v>
       </c>
       <c r="N33" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O33" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="P33" s="1" t="n">
         <v>2</v>
@@ -4100,13 +4100,13 @@
         <v>-2</v>
       </c>
       <c r="AC33" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD33" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE33" s="1" t="n">
-        <v>33.33</v>
+        <v>50</v>
       </c>
       <c r="AF33" s="1" t="n">
         <v>0</v>
@@ -4118,25 +4118,25 @@
         <v>2</v>
       </c>
       <c r="AI33" s="1" t="n">
-        <v>66.67</v>
+        <v>50</v>
       </c>
       <c r="AJ33" s="1" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AK33" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="AL33" s="1" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="AM33" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO33" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="AL33" s="1" t="n">
-        <v>1.67</v>
-      </c>
-      <c r="AM33" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AN33" s="1" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="AO33" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -4151,10 +4151,10 @@
         </is>
       </c>
       <c r="C34" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E34" s="1" t="n">
         <v>100</v>
@@ -4175,67 +4175,67 @@
         <v>3</v>
       </c>
       <c r="K34" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="L34" s="1" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="M34" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="N34" s="1" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="O34" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="L34" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="M34" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="N34" s="1" t="n">
+      <c r="P34" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R34" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="S34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V34" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="W34" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="O34" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="P34" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U34" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="V34" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="W34" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="X34" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y34" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z34" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AB34" s="1" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC34" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AD34" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE34" s="1" t="n">
-        <v>66.67</v>
+        <v>80</v>
       </c>
       <c r="AF34" s="1" t="n">
         <v>0</v>
@@ -4247,25 +4247,25 @@
         <v>1</v>
       </c>
       <c r="AI34" s="1" t="n">
-        <v>33.33</v>
+        <v>20</v>
       </c>
       <c r="AJ34" s="1" t="n">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="AK34" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="AL34" s="1" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="AM34" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="AN34" s="1" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AO34" s="1" t="n">
         <v>6</v>
-      </c>
-      <c r="AL34" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM34" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AN34" s="1" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="AO34" s="1" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -4280,13 +4280,13 @@
         </is>
       </c>
       <c r="C35" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>50</v>
+        <v>66.67</v>
       </c>
       <c r="F35" s="1" t="n">
         <v>0</v>
@@ -4298,28 +4298,28 @@
         <v>1</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>50</v>
+        <v>33.33</v>
       </c>
       <c r="J35" s="1" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="K35" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L35" s="1" t="n">
-        <v>1.5</v>
+        <v>1.33</v>
       </c>
       <c r="M35" s="1" t="n">
         <v>2</v>
       </c>
       <c r="N35" s="1" t="n">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="O35" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P35" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q35" s="1" t="n">
         <v>0</v>
@@ -4334,7 +4334,7 @@
         <v>0</v>
       </c>
       <c r="U35" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V35" s="1" t="n">
         <v>100</v>
@@ -4343,28 +4343,28 @@
         <v>0</v>
       </c>
       <c r="X35" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="Z35" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AA35" s="1" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AB35" s="1" t="n">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="AC35" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AD35" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE35" s="1" t="n">
-        <v>33.33</v>
+        <v>40</v>
       </c>
       <c r="AF35" s="1" t="n">
         <v>0</v>
@@ -4373,28 +4373,28 @@
         <v>0</v>
       </c>
       <c r="AH35" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI35" s="1" t="n">
-        <v>66.67</v>
+        <v>60</v>
       </c>
       <c r="AJ35" s="1" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="AK35" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AL35" s="1" t="n">
-        <v>1.33</v>
+        <v>1.2</v>
       </c>
       <c r="AM35" s="1" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AN35" s="1" t="n">
-        <v>1.67</v>
+        <v>1.8</v>
       </c>
       <c r="AO35" s="1" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="36">
@@ -4409,10 +4409,10 @@
         </is>
       </c>
       <c r="C36" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" s="1" t="n">
         <v>100</v>
@@ -4433,10 +4433,10 @@
         <v>3</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L36" s="1" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="M36" s="1" t="n">
         <v>0</v>
@@ -4445,7 +4445,7 @@
         <v>0</v>
       </c>
       <c r="O36" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P36" s="1" t="n">
         <v>2</v>
@@ -4487,10 +4487,10 @@
         <v>4</v>
       </c>
       <c r="AC36" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD36" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE36" s="1" t="n">
         <v>100</v>
@@ -4511,19 +4511,19 @@
         <v>3</v>
       </c>
       <c r="AK36" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AL36" s="1" t="n">
-        <v>2.67</v>
+        <v>2.5</v>
       </c>
       <c r="AM36" s="1" t="n">
         <v>3</v>
       </c>
       <c r="AN36" s="1" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AO36" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update GW 16 2025/26
</commit_message>
<xml_diff>
--- a/app/football_statistics_2025_26.xlsx
+++ b/app/football_statistics_2025_26.xlsx
@@ -695,19 +695,19 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>83.33</v>
+        <v>87.5</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>16.67</v>
+        <v>12.5</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0</v>
@@ -716,100 +716,100 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>2.67</v>
+        <v>2.75</v>
       </c>
       <c r="K2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="V2" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA2" s="1" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="AB2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="L2" s="1" t="n">
-        <v>2.67</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="N2" s="1" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>57.14</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="T2" s="1" t="n">
-        <v>28.57</v>
-      </c>
-      <c r="U2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="V2" s="1" t="n">
-        <v>14.29</v>
-      </c>
-      <c r="W2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="X2" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="Y2" s="1" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="Z2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AA2" s="1" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="AB2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AC2" s="1" t="n">
-        <v>13</v>
-      </c>
       <c r="AD2" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AE2" s="1" t="n">
-        <v>69.23</v>
+        <v>68.75</v>
       </c>
       <c r="AF2" s="1" t="n">
         <v>3</v>
       </c>
       <c r="AG2" s="1" t="n">
-        <v>23.08</v>
+        <v>18.75</v>
       </c>
       <c r="AH2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI2" s="1" t="n">
-        <v>7.69</v>
+        <v>12.5</v>
       </c>
       <c r="AJ2" s="1" t="n">
-        <v>2.31</v>
+        <v>2.25</v>
       </c>
       <c r="AK2" s="1" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="AL2" s="1" t="n">
-        <v>1.92</v>
+        <v>1.88</v>
       </c>
       <c r="AM2" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AN2" s="1" t="n">
-        <v>0.54</v>
+        <v>0.62</v>
       </c>
       <c r="AO2" s="1" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -824,118 +824,118 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>42.86</v>
+        <v>50</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>28.57</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>28.57</v>
+        <v>25</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>1.57</v>
+        <v>1.75</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>1.43</v>
+        <v>1.5</v>
       </c>
       <c r="M3" s="1" t="n">
         <v>7</v>
       </c>
       <c r="N3" s="1" t="n">
-        <v>1</v>
+        <v>0.88</v>
       </c>
       <c r="O3" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P3" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q3" s="1" t="n">
         <v>4</v>
       </c>
       <c r="R3" s="1" t="n">
-        <v>66.67</v>
+        <v>50</v>
       </c>
       <c r="S3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T3" s="1" t="n">
-        <v>16.67</v>
+        <v>25</v>
       </c>
       <c r="U3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V3" s="1" t="n">
-        <v>16.67</v>
+        <v>25</v>
       </c>
       <c r="W3" s="1" t="n">
-        <v>2.17</v>
+        <v>1.75</v>
       </c>
       <c r="X3" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Y3" s="1" t="n">
-        <v>2.33</v>
+        <v>1.88</v>
       </c>
       <c r="Z3" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AA3" s="1" t="n">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="AB3" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC3" s="1" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AD3" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE3" s="1" t="n">
-        <v>53.85</v>
+        <v>50</v>
       </c>
       <c r="AF3" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG3" s="1" t="n">
-        <v>23.08</v>
+        <v>25</v>
       </c>
       <c r="AH3" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AI3" s="1" t="n">
-        <v>23.08</v>
+        <v>25</v>
       </c>
       <c r="AJ3" s="1" t="n">
-        <v>1.85</v>
+        <v>1.75</v>
       </c>
       <c r="AK3" s="1" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="AL3" s="1" t="n">
-        <v>1.85</v>
+        <v>1.69</v>
       </c>
       <c r="AM3" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AN3" s="1" t="n">
-        <v>0.92</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="AO3" s="1" t="n">
         <v>12</v>
@@ -953,121 +953,121 @@
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>66.67</v>
+        <v>62.5</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>33.33</v>
+        <v>25</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>1.67</v>
+        <v>1.62</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N4" s="1" t="n">
-        <v>1.33</v>
+        <v>1.12</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P4" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="R4" s="1" t="n">
-        <v>42.86</v>
+        <v>37.5</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4" s="1" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="U4" s="1" t="n">
         <v>4</v>
       </c>
       <c r="V4" s="1" t="n">
-        <v>57.14</v>
+        <v>50</v>
       </c>
       <c r="W4" s="1" t="n">
-        <v>1.29</v>
+        <v>1.25</v>
       </c>
       <c r="X4" s="1" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="Y4" s="1" t="n">
-        <v>1.43</v>
+        <v>1.62</v>
       </c>
       <c r="Z4" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AA4" s="1" t="n">
-        <v>1.71</v>
+        <v>1.88</v>
       </c>
       <c r="AB4" s="1" t="n">
         <v>-2</v>
       </c>
       <c r="AC4" s="1" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AD4" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE4" s="1" t="n">
-        <v>53.85</v>
+        <v>50</v>
       </c>
       <c r="AF4" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG4" s="1" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="AH4" s="1" t="n">
         <v>6</v>
       </c>
       <c r="AI4" s="1" t="n">
-        <v>46.15</v>
+        <v>37.5</v>
       </c>
       <c r="AJ4" s="1" t="n">
         <v>1.62</v>
       </c>
       <c r="AK4" s="1" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="AL4" s="1" t="n">
-        <v>1.54</v>
+        <v>1.62</v>
       </c>
       <c r="AM4" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="AN4" s="1" t="n">
-        <v>1.54</v>
+        <v>1.5</v>
       </c>
       <c r="AO4" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -1082,13 +1082,13 @@
         </is>
       </c>
       <c r="C5" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>6</v>
-      </c>
       <c r="E5" s="1" t="n">
-        <v>85.70999999999999</v>
+        <v>87.5</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>0</v>
@@ -1100,103 +1100,103 @@
         <v>1</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>2.57</v>
+        <v>2.63</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>2.71</v>
+        <v>2.75</v>
       </c>
       <c r="M5" s="1" t="n">
         <v>6</v>
       </c>
       <c r="N5" s="1" t="n">
-        <v>0.86</v>
+        <v>0.75</v>
       </c>
       <c r="O5" s="1" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="P5" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q5" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R5" s="1" t="n">
-        <v>33.33</v>
+        <v>50</v>
       </c>
       <c r="S5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T5" s="1" t="n">
-        <v>16.67</v>
+        <v>12.5</v>
       </c>
       <c r="U5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="V5" s="1" t="n">
-        <v>50</v>
+        <v>37.5</v>
       </c>
       <c r="W5" s="1" t="n">
-        <v>1.17</v>
+        <v>1.63</v>
       </c>
       <c r="X5" s="1" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="Y5" s="1" t="n">
-        <v>1.33</v>
+        <v>2</v>
       </c>
       <c r="Z5" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA5" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AB5" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="AA5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="AC5" s="1" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AD5" s="1" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="AE5" s="1" t="n">
-        <v>61.54</v>
+        <v>68.75</v>
       </c>
       <c r="AF5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AG5" s="1" t="n">
-        <v>7.69</v>
+        <v>6.25</v>
       </c>
       <c r="AH5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="AI5" s="1" t="n">
-        <v>30.77</v>
+        <v>25</v>
       </c>
       <c r="AJ5" s="1" t="n">
-        <v>1.92</v>
+        <v>2.12</v>
       </c>
       <c r="AK5" s="1" t="n">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="AL5" s="1" t="n">
-        <v>2.08</v>
+        <v>2.38</v>
       </c>
       <c r="AM5" s="1" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="AN5" s="1" t="n">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="AO5" s="1" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
@@ -1211,121 +1211,121 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>66.67</v>
+        <v>57.14</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>0</v>
+        <v>14.29</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>33.33</v>
+        <v>28.57</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>2</v>
+        <v>1.86</v>
       </c>
       <c r="K6" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>1.83</v>
+        <v>1.71</v>
       </c>
       <c r="M6" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N6" s="1" t="n">
-        <v>1.17</v>
+        <v>1.14</v>
       </c>
       <c r="O6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="P6" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q6" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R6" s="1" t="n">
-        <v>28.57</v>
+        <v>37.5</v>
       </c>
       <c r="S6" s="1" t="n">
         <v>3</v>
       </c>
       <c r="T6" s="1" t="n">
-        <v>42.86</v>
+        <v>37.5</v>
       </c>
       <c r="U6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="V6" s="1" t="n">
-        <v>28.57</v>
+        <v>25</v>
       </c>
       <c r="W6" s="1" t="n">
-        <v>1.29</v>
+        <v>1.5</v>
       </c>
       <c r="X6" s="1" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="Y6" s="1" t="n">
-        <v>1.43</v>
+        <v>1.75</v>
       </c>
       <c r="Z6" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AA6" s="1" t="n">
-        <v>1.86</v>
+        <v>1.75</v>
       </c>
       <c r="AB6" s="1" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="1" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AD6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE6" s="1" t="n">
-        <v>46.15</v>
+        <v>46.67</v>
       </c>
       <c r="AF6" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG6" s="1" t="n">
-        <v>23.08</v>
+        <v>26.67</v>
       </c>
       <c r="AH6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="AI6" s="1" t="n">
-        <v>30.77</v>
+        <v>26.67</v>
       </c>
       <c r="AJ6" s="1" t="n">
-        <v>1.62</v>
+        <v>1.67</v>
       </c>
       <c r="AK6" s="1" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="AL6" s="1" t="n">
-        <v>1.62</v>
+        <v>1.73</v>
       </c>
       <c r="AM6" s="1" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AN6" s="1" t="n">
-        <v>1.54</v>
+        <v>1.47</v>
       </c>
       <c r="AO6" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -1430,121 +1430,121 @@
         </is>
       </c>
       <c r="C9" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>88.89</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>2.78</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="M9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E9" s="1" t="n">
-        <v>87.5</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="H9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1" t="n">
-        <v>2.75</v>
-      </c>
-      <c r="K9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="L9" s="1" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="M9" s="1" t="n">
-        <v>6</v>
-      </c>
       <c r="N9" s="1" t="n">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
       <c r="O9" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P9" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R9" s="1" t="n">
-        <v>33.33</v>
+        <v>25</v>
       </c>
       <c r="S9" s="1" t="n">
         <v>3</v>
       </c>
       <c r="T9" s="1" t="n">
-        <v>50</v>
+        <v>37.5</v>
       </c>
       <c r="U9" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>16.67</v>
+        <v>37.5</v>
       </c>
       <c r="W9" s="1" t="n">
-        <v>1.5</v>
+        <v>1.13</v>
       </c>
       <c r="X9" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Y9" s="1" t="n">
-        <v>1.17</v>
+        <v>1</v>
       </c>
       <c r="Z9" s="1" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AA9" s="1" t="n">
-        <v>0.83</v>
+        <v>1.12</v>
       </c>
       <c r="AB9" s="1" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AC9" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AD9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE9" s="1" t="n">
+        <v>58.82</v>
+      </c>
+      <c r="AF9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG9" s="1" t="n">
+        <v>23.53</v>
+      </c>
+      <c r="AH9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI9" s="1" t="n">
+        <v>17.65</v>
+      </c>
+      <c r="AJ9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK9" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AL9" s="1" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="AM9" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AN9" s="1" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="AO9" s="1" t="n">
         <v>14</v>
-      </c>
-      <c r="AD9" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="AE9" s="1" t="n">
-        <v>64.29000000000001</v>
-      </c>
-      <c r="AF9" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AG9" s="1" t="n">
-        <v>28.57</v>
-      </c>
-      <c r="AH9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI9" s="1" t="n">
-        <v>7.14</v>
-      </c>
-      <c r="AJ9" s="1" t="n">
-        <v>2.21</v>
-      </c>
-      <c r="AK9" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="AL9" s="1" t="n">
-        <v>1.93</v>
-      </c>
-      <c r="AM9" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="AN9" s="1" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="AO9" s="1" t="n">
-        <v>16</v>
       </c>
     </row>
     <row r="10">
@@ -1559,10 +1559,10 @@
         </is>
       </c>
       <c r="C10" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>100</v>
@@ -1583,97 +1583,97 @@
         <v>3</v>
       </c>
       <c r="K10" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="O10" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="L10" s="1" t="n">
-        <v>3.29</v>
-      </c>
-      <c r="M10" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="N10" s="1" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="O10" s="1" t="n">
-        <v>19</v>
-      </c>
       <c r="P10" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q10" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R10" s="1" t="n">
-        <v>57.14</v>
+        <v>62.5</v>
       </c>
       <c r="S10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T10" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="U10" s="1" t="n">
         <v>2</v>
       </c>
       <c r="V10" s="1" t="n">
-        <v>28.57</v>
+        <v>25</v>
       </c>
       <c r="W10" s="1" t="n">
-        <v>1.86</v>
+        <v>2</v>
       </c>
       <c r="X10" s="1" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="Y10" s="1" t="n">
-        <v>2.29</v>
+        <v>2.62</v>
       </c>
       <c r="Z10" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AA10" s="1" t="n">
-        <v>1.71</v>
+        <v>1.88</v>
       </c>
       <c r="AB10" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AC10" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AD10" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="AD10" s="1" t="n">
-        <v>11</v>
-      </c>
       <c r="AE10" s="1" t="n">
-        <v>78.56999999999999</v>
+        <v>82.34999999999999</v>
       </c>
       <c r="AF10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AG10" s="1" t="n">
-        <v>7.14</v>
+        <v>5.88</v>
       </c>
       <c r="AH10" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AI10" s="1" t="n">
-        <v>14.29</v>
+        <v>11.76</v>
       </c>
       <c r="AJ10" s="1" t="n">
-        <v>2.43</v>
+        <v>2.53</v>
       </c>
       <c r="AK10" s="1" t="n">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="AL10" s="1" t="n">
-        <v>2.79</v>
+        <v>2.88</v>
       </c>
       <c r="AM10" s="1" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AN10" s="1" t="n">
-        <v>1.14</v>
+        <v>1.18</v>
       </c>
       <c r="AO10" s="1" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
@@ -1688,13 +1688,13 @@
         </is>
       </c>
       <c r="C11" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>6</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>100</v>
+        <v>85.70999999999999</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>0</v>
@@ -1703,106 +1703,106 @@
         <v>0</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>0</v>
+        <v>14.29</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>3</v>
+        <v>2.57</v>
       </c>
       <c r="K11" s="1" t="n">
         <v>14</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>2.33</v>
+        <v>2</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>0.5</v>
+        <v>0.71</v>
       </c>
       <c r="O11" s="1" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q11" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R11" s="1" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="S11" s="1" t="n">
         <v>3</v>
       </c>
       <c r="T11" s="1" t="n">
-        <v>37.5</v>
+        <v>30</v>
       </c>
       <c r="U11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="W11" s="1" t="n">
-        <v>1.88</v>
+        <v>2.1</v>
       </c>
       <c r="X11" s="1" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Y11" s="1" t="n">
-        <v>1.88</v>
+        <v>2</v>
       </c>
       <c r="Z11" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AA11" s="1" t="n">
-        <v>1.25</v>
+        <v>1.1</v>
       </c>
       <c r="AB11" s="1" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AC11" s="1" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="AD11" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AE11" s="1" t="n">
-        <v>71.43000000000001</v>
+        <v>70.59</v>
       </c>
       <c r="AF11" s="1" t="n">
         <v>3</v>
       </c>
       <c r="AG11" s="1" t="n">
-        <v>21.43</v>
+        <v>17.65</v>
       </c>
       <c r="AH11" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI11" s="1" t="n">
-        <v>7.14</v>
+        <v>11.76</v>
       </c>
       <c r="AJ11" s="1" t="n">
-        <v>2.36</v>
+        <v>2.29</v>
       </c>
       <c r="AK11" s="1" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="AL11" s="1" t="n">
-        <v>2.07</v>
+        <v>2</v>
       </c>
       <c r="AM11" s="1" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AN11" s="1" t="n">
-        <v>0.93</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="AO11" s="1" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
@@ -1907,118 +1907,118 @@
         </is>
       </c>
       <c r="C14" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>57.14</v>
+        <v>62.5</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>28.57</v>
+        <v>25</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>1.86</v>
+        <v>2</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L14" s="1" t="n">
-        <v>2.29</v>
+        <v>2.25</v>
       </c>
       <c r="M14" s="1" t="n">
         <v>6</v>
       </c>
       <c r="N14" s="1" t="n">
-        <v>0.86</v>
+        <v>0.75</v>
       </c>
       <c r="O14" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q14" s="1" t="n">
         <v>3</v>
       </c>
       <c r="R14" s="1" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="S14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T14" s="1" t="n">
-        <v>20</v>
+        <v>16.67</v>
       </c>
       <c r="U14" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>20</v>
+        <v>33.33</v>
       </c>
       <c r="W14" s="1" t="n">
-        <v>2</v>
+        <v>1.67</v>
       </c>
       <c r="X14" s="1" t="n">
         <v>12</v>
       </c>
       <c r="Y14" s="1" t="n">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="Z14" s="1" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AA14" s="1" t="n">
-        <v>2.2</v>
+        <v>2.17</v>
       </c>
       <c r="AB14" s="1" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC14" s="1" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AD14" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE14" s="1" t="n">
-        <v>58.33</v>
+        <v>57.14</v>
       </c>
       <c r="AF14" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AG14" s="1" t="n">
-        <v>16.67</v>
+        <v>14.29</v>
       </c>
       <c r="AH14" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AI14" s="1" t="n">
-        <v>25</v>
+        <v>28.57</v>
       </c>
       <c r="AJ14" s="1" t="n">
-        <v>1.92</v>
+        <v>1.86</v>
       </c>
       <c r="AK14" s="1" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="AL14" s="1" t="n">
-        <v>2.33</v>
+        <v>2.14</v>
       </c>
       <c r="AM14" s="1" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AN14" s="1" t="n">
-        <v>1.42</v>
+        <v>1.36</v>
       </c>
       <c r="AO14" s="1" t="n">
         <v>11</v>
@@ -2036,19 +2036,19 @@
         </is>
       </c>
       <c r="C15" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>7</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>100</v>
+        <v>87.5</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>0</v>
@@ -2057,100 +2057,100 @@
         <v>0</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L15" s="1" t="n">
-        <v>4.14</v>
+        <v>3.88</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>0.57</v>
+        <v>0.75</v>
       </c>
       <c r="O15" s="1" t="n">
         <v>25</v>
       </c>
       <c r="P15" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="Q15" s="1" t="n">
-        <v>4</v>
-      </c>
       <c r="R15" s="1" t="n">
-        <v>80</v>
+        <v>83.33</v>
       </c>
       <c r="S15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T15" s="1" t="n">
+        <v>16.67</v>
+      </c>
+      <c r="U15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" s="1" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="X15" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="U15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W15" s="1" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="X15" s="1" t="n">
-        <v>15</v>
-      </c>
       <c r="Y15" s="1" t="n">
-        <v>3</v>
+        <v>3.33</v>
       </c>
       <c r="Z15" s="1" t="n">
         <v>5</v>
       </c>
       <c r="AA15" s="1" t="n">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="AB15" s="1" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AC15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD15" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="AD15" s="1" t="n">
+      <c r="AE15" s="1" t="n">
+        <v>85.70999999999999</v>
+      </c>
+      <c r="AF15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG15" s="1" t="n">
+        <v>14.29</v>
+      </c>
+      <c r="AH15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="1" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="AK15" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="AL15" s="1" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="AM15" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="AE15" s="1" t="n">
-        <v>91.67</v>
-      </c>
-      <c r="AF15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG15" s="1" t="n">
-        <v>8.33</v>
-      </c>
-      <c r="AH15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="1" t="n">
-        <v>2.83</v>
-      </c>
-      <c r="AK15" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="AL15" s="1" t="n">
-        <v>3.67</v>
-      </c>
-      <c r="AM15" s="1" t="n">
-        <v>9</v>
-      </c>
       <c r="AN15" s="1" t="n">
-        <v>0.75</v>
+        <v>0.79</v>
       </c>
       <c r="AO15" s="1" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16">
@@ -2165,76 +2165,76 @@
         </is>
       </c>
       <c r="C16" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="O16" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="P16" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="R16" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="S16" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E16" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="F16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="H16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="K16" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="L16" s="1" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="M16" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="N16" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="O16" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="P16" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="Q16" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="R16" s="1" t="n">
-        <v>57.14</v>
-      </c>
-      <c r="S16" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="T16" s="1" t="n">
-        <v>28.57</v>
+        <v>37.5</v>
       </c>
       <c r="U16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="V16" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="W16" s="1" t="n">
-        <v>2</v>
+        <v>1.88</v>
       </c>
       <c r="X16" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Y16" s="1" t="n">
-        <v>1.71</v>
+        <v>1.62</v>
       </c>
       <c r="Z16" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AA16" s="1" t="n">
         <v>1</v>
@@ -2243,43 +2243,43 @@
         <v>5</v>
       </c>
       <c r="AC16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD16" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE16" s="1" t="n">
+        <v>57.14</v>
+      </c>
+      <c r="AF16" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG16" s="1" t="n">
+        <v>35.71</v>
+      </c>
+      <c r="AH16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI16" s="1" t="n">
+        <v>7.14</v>
+      </c>
+      <c r="AJ16" s="1" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="AK16" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AL16" s="1" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="AM16" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="AD16" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="AE16" s="1" t="n">
-        <v>58.33</v>
-      </c>
-      <c r="AF16" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AG16" s="1" t="n">
-        <v>33.33</v>
-      </c>
-      <c r="AH16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI16" s="1" t="n">
-        <v>8.33</v>
-      </c>
-      <c r="AJ16" s="1" t="n">
-        <v>2.08</v>
-      </c>
-      <c r="AK16" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="AL16" s="1" t="n">
-        <v>1.75</v>
-      </c>
-      <c r="AM16" s="1" t="n">
-        <v>11</v>
-      </c>
       <c r="AN16" s="1" t="n">
-        <v>0.92</v>
+        <v>0.86</v>
       </c>
       <c r="AO16" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -2294,88 +2294,88 @@
         </is>
       </c>
       <c r="C17" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>50</v>
+        <v>57.14</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>16.67</v>
+        <v>14.29</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>33.33</v>
+        <v>28.57</v>
       </c>
       <c r="J17" s="1" t="n">
-        <v>1.67</v>
+        <v>1.86</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L17" s="1" t="n">
-        <v>1.83</v>
+        <v>1.71</v>
       </c>
       <c r="M17" s="1" t="n">
         <v>9</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>1.5</v>
+        <v>1.29</v>
       </c>
       <c r="O17" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P17" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q17" s="1" t="n">
         <v>3</v>
       </c>
       <c r="R17" s="1" t="n">
-        <v>50</v>
+        <v>42.86</v>
       </c>
       <c r="S17" s="1" t="n">
         <v>2</v>
       </c>
       <c r="T17" s="1" t="n">
-        <v>33.33</v>
+        <v>28.57</v>
       </c>
       <c r="U17" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V17" s="1" t="n">
-        <v>16.67</v>
+        <v>28.57</v>
       </c>
       <c r="W17" s="1" t="n">
-        <v>1.83</v>
+        <v>1.57</v>
       </c>
       <c r="X17" s="1" t="n">
         <v>17</v>
       </c>
       <c r="Y17" s="1" t="n">
-        <v>2.83</v>
+        <v>2.43</v>
       </c>
       <c r="Z17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA17" s="1" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="AB17" s="1" t="n">
+        <v>-3</v>
+      </c>
+      <c r="AC17" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="AA17" s="1" t="n">
-        <v>2.33</v>
-      </c>
-      <c r="AB17" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC17" s="1" t="n">
-        <v>12</v>
-      </c>
       <c r="AD17" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE17" s="1" t="n">
         <v>50</v>
@@ -2384,31 +2384,31 @@
         <v>3</v>
       </c>
       <c r="AG17" s="1" t="n">
-        <v>25</v>
+        <v>21.43</v>
       </c>
       <c r="AH17" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AI17" s="1" t="n">
-        <v>25</v>
+        <v>28.57</v>
       </c>
       <c r="AJ17" s="1" t="n">
-        <v>1.75</v>
+        <v>1.71</v>
       </c>
       <c r="AK17" s="1" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AL17" s="1" t="n">
-        <v>2.33</v>
+        <v>2.07</v>
       </c>
       <c r="AM17" s="1" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="AN17" s="1" t="n">
-        <v>1.92</v>
+        <v>2.07</v>
       </c>
       <c r="AO17" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -2423,7 +2423,7 @@
         </is>
       </c>
       <c r="C18" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>0</v>
@@ -2435,109 +2435,109 @@
         <v>2</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>33.33</v>
+        <v>28.57</v>
       </c>
       <c r="H18" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>66.67</v>
+        <v>71.43000000000001</v>
       </c>
       <c r="J18" s="1" t="n">
-        <v>0.33</v>
+        <v>0.29</v>
       </c>
       <c r="K18" s="1" t="n">
         <v>5</v>
       </c>
       <c r="L18" s="1" t="n">
-        <v>0.83</v>
+        <v>0.71</v>
       </c>
       <c r="M18" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N18" s="1" t="n">
-        <v>1.67</v>
+        <v>1.57</v>
       </c>
       <c r="O18" s="1" t="n">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="P18" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R18" s="1" t="n">
-        <v>16.67</v>
+        <v>14.29</v>
       </c>
       <c r="S18" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T18" s="1" t="n">
-        <v>16.67</v>
+        <v>28.57</v>
       </c>
       <c r="U18" s="1" t="n">
         <v>4</v>
       </c>
       <c r="V18" s="1" t="n">
-        <v>66.67</v>
+        <v>57.14</v>
       </c>
       <c r="W18" s="1" t="n">
-        <v>0.67</v>
+        <v>0.71</v>
       </c>
       <c r="X18" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Y18" s="1" t="n">
-        <v>1</v>
+        <v>1.14</v>
       </c>
       <c r="Z18" s="1" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AA18" s="1" t="n">
-        <v>2.17</v>
+        <v>2.14</v>
       </c>
       <c r="AB18" s="1" t="n">
         <v>-7</v>
       </c>
       <c r="AC18" s="1" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AD18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AE18" s="1" t="n">
-        <v>8.33</v>
+        <v>7.14</v>
       </c>
       <c r="AF18" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG18" s="1" t="n">
-        <v>25</v>
+        <v>28.57</v>
       </c>
       <c r="AH18" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AI18" s="1" t="n">
-        <v>66.67</v>
+        <v>64.29000000000001</v>
       </c>
       <c r="AJ18" s="1" t="n">
         <v>0.5</v>
       </c>
       <c r="AK18" s="1" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AL18" s="1" t="n">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="AM18" s="1" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="AN18" s="1" t="n">
-        <v>1.92</v>
+        <v>1.86</v>
       </c>
       <c r="AO18" s="1" t="n">
-        <v>-12</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="19">
@@ -2552,10 +2552,10 @@
         </is>
       </c>
       <c r="C19" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>100</v>
@@ -2576,97 +2576,97 @@
         <v>3</v>
       </c>
       <c r="K19" s="1" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="L19" s="1" t="n">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="M19" s="1" t="n">
         <v>3</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="O19" s="1" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="P19" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="1" t="n">
         <v>3</v>
       </c>
       <c r="R19" s="1" t="n">
-        <v>42.86</v>
+        <v>37.5</v>
       </c>
       <c r="S19" s="1" t="n">
         <v>2</v>
       </c>
       <c r="T19" s="1" t="n">
-        <v>28.57</v>
+        <v>25</v>
       </c>
       <c r="U19" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V19" s="1" t="n">
-        <v>28.57</v>
+        <v>37.5</v>
       </c>
       <c r="W19" s="1" t="n">
-        <v>1.57</v>
+        <v>1.38</v>
       </c>
       <c r="X19" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Y19" s="1" t="n">
-        <v>1.43</v>
+        <v>1.38</v>
       </c>
       <c r="Z19" s="1" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AA19" s="1" t="n">
-        <v>1.43</v>
+        <v>1.62</v>
       </c>
       <c r="AB19" s="1" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="AC19" s="1" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AD19" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AE19" s="1" t="n">
-        <v>66.67</v>
+        <v>64.29000000000001</v>
       </c>
       <c r="AF19" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AG19" s="1" t="n">
-        <v>16.67</v>
+        <v>14.29</v>
       </c>
       <c r="AH19" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI19" s="1" t="n">
-        <v>16.67</v>
+        <v>21.43</v>
       </c>
       <c r="AJ19" s="1" t="n">
-        <v>2.17</v>
+        <v>2.07</v>
       </c>
       <c r="AK19" s="1" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="AL19" s="1" t="n">
-        <v>1.83</v>
+        <v>2.07</v>
       </c>
       <c r="AM19" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AN19" s="1" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="AO19" s="1" t="n">
         <v>13</v>
-      </c>
-      <c r="AN19" s="1" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="AO19" s="1" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="20">
@@ -2681,13 +2681,13 @@
         </is>
       </c>
       <c r="C20" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>100</v>
+        <v>83.33</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>0</v>
@@ -2696,106 +2696,106 @@
         <v>0</v>
       </c>
       <c r="H20" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>0</v>
+        <v>16.67</v>
       </c>
       <c r="J20" s="1" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="K20" s="1" t="n">
         <v>9</v>
       </c>
       <c r="L20" s="1" t="n">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="M20" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="N20" s="1" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="O20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P20" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q20" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="N20" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="O20" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="P20" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="Q20" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="R20" s="1" t="n">
-        <v>28.57</v>
+        <v>37.5</v>
       </c>
       <c r="S20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T20" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="U20" s="1" t="n">
         <v>4</v>
       </c>
       <c r="V20" s="1" t="n">
-        <v>57.14</v>
+        <v>50</v>
       </c>
       <c r="W20" s="1" t="n">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="X20" s="1" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Y20" s="1" t="n">
-        <v>1.71</v>
+        <v>2</v>
       </c>
       <c r="Z20" s="1" t="n">
         <v>14</v>
       </c>
       <c r="AA20" s="1" t="n">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="AB20" s="1" t="n">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="AC20" s="1" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AD20" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE20" s="1" t="n">
-        <v>58.33</v>
+        <v>57.14</v>
       </c>
       <c r="AF20" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AG20" s="1" t="n">
-        <v>8.33</v>
+        <v>7.14</v>
       </c>
       <c r="AH20" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI20" s="1" t="n">
-        <v>33.33</v>
+        <v>35.71</v>
       </c>
       <c r="AJ20" s="1" t="n">
-        <v>1.83</v>
+        <v>1.79</v>
       </c>
       <c r="AK20" s="1" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="AL20" s="1" t="n">
-        <v>1.75</v>
+        <v>1.79</v>
       </c>
       <c r="AM20" s="1" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="AN20" s="1" t="n">
-        <v>1.42</v>
+        <v>1.57</v>
       </c>
       <c r="AO20" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -2900,58 +2900,58 @@
         </is>
       </c>
       <c r="C23" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>71.43000000000001</v>
+        <v>62.5</v>
       </c>
       <c r="F23" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>14.29</v>
+        <v>25</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="J23" s="1" t="n">
-        <v>2.29</v>
+        <v>2.13</v>
       </c>
       <c r="K23" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L23" s="1" t="n">
-        <v>1.43</v>
+        <v>1.5</v>
       </c>
       <c r="M23" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N23" s="1" t="n">
-        <v>0.86</v>
+        <v>1</v>
       </c>
       <c r="O23" s="1" t="n">
         <v>4</v>
       </c>
       <c r="P23" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R23" s="1" t="n">
-        <v>50</v>
+        <v>57.14</v>
       </c>
       <c r="S23" s="1" t="n">
         <v>3</v>
       </c>
       <c r="T23" s="1" t="n">
-        <v>50</v>
+        <v>42.86</v>
       </c>
       <c r="U23" s="1" t="n">
         <v>0</v>
@@ -2960,61 +2960,61 @@
         <v>0</v>
       </c>
       <c r="W23" s="1" t="n">
-        <v>2</v>
+        <v>2.14</v>
       </c>
       <c r="X23" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y23" s="1" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="Z23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA23" s="1" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="AB23" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC23" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="AD23" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="Y23" s="1" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="Z23" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA23" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AB23" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="AC23" s="1" t="n">
+      <c r="AE23" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="AF23" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG23" s="1" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="AH23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI23" s="1" t="n">
+        <v>6.67</v>
+      </c>
+      <c r="AJ23" s="1" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="AK23" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AL23" s="1" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="AM23" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="AD23" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="AE23" s="1" t="n">
-        <v>61.54</v>
-      </c>
-      <c r="AF23" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AG23" s="1" t="n">
-        <v>30.77</v>
-      </c>
-      <c r="AH23" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI23" s="1" t="n">
-        <v>7.69</v>
-      </c>
-      <c r="AJ23" s="1" t="n">
-        <v>2.15</v>
-      </c>
-      <c r="AK23" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="AL23" s="1" t="n">
-        <v>1.46</v>
-      </c>
-      <c r="AM23" s="1" t="n">
-        <v>9</v>
-      </c>
       <c r="AN23" s="1" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.87</v>
       </c>
       <c r="AO23" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24">
@@ -3029,13 +3029,13 @@
         </is>
       </c>
       <c r="C24" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>71.43000000000001</v>
+        <v>75</v>
       </c>
       <c r="F24" s="1" t="n">
         <v>0</v>
@@ -3047,34 +3047,34 @@
         <v>2</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>28.57</v>
+        <v>25</v>
       </c>
       <c r="J24" s="1" t="n">
-        <v>2.14</v>
+        <v>2.25</v>
       </c>
       <c r="K24" s="1" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="L24" s="1" t="n">
-        <v>2.43</v>
+        <v>2.62</v>
       </c>
       <c r="M24" s="1" t="n">
         <v>5</v>
       </c>
       <c r="N24" s="1" t="n">
-        <v>0.71</v>
+        <v>0.62</v>
       </c>
       <c r="O24" s="1" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="P24" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R24" s="1" t="n">
-        <v>66.67</v>
+        <v>71.43000000000001</v>
       </c>
       <c r="S24" s="1" t="n">
         <v>0</v>
@@ -3086,34 +3086,34 @@
         <v>2</v>
       </c>
       <c r="V24" s="1" t="n">
-        <v>33.33</v>
+        <v>28.57</v>
       </c>
       <c r="W24" s="1" t="n">
-        <v>2</v>
+        <v>2.14</v>
       </c>
       <c r="X24" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="Y24" s="1" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="Z24" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA24" s="1" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="AB24" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC24" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="AD24" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="Y24" s="1" t="n">
-        <v>1.83</v>
-      </c>
-      <c r="Z24" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="AA24" s="1" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="AB24" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC24" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="AD24" s="1" t="n">
-        <v>9</v>
-      </c>
       <c r="AE24" s="1" t="n">
-        <v>69.23</v>
+        <v>73.33</v>
       </c>
       <c r="AF24" s="1" t="n">
         <v>0</v>
@@ -3125,25 +3125,25 @@
         <v>4</v>
       </c>
       <c r="AI24" s="1" t="n">
-        <v>30.77</v>
+        <v>26.67</v>
       </c>
       <c r="AJ24" s="1" t="n">
-        <v>2.08</v>
+        <v>2.2</v>
       </c>
       <c r="AK24" s="1" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="AL24" s="1" t="n">
-        <v>2.15</v>
+        <v>2.27</v>
       </c>
       <c r="AM24" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AN24" s="1" t="n">
-        <v>1</v>
+        <v>0.93</v>
       </c>
       <c r="AO24" s="1" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25">
@@ -3197,37 +3197,37 @@
         <v>6</v>
       </c>
       <c r="P25" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q25" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R25" s="1" t="n">
-        <v>33.33</v>
+        <v>37.5</v>
       </c>
       <c r="S25" s="1" t="n">
         <v>2</v>
       </c>
       <c r="T25" s="1" t="n">
-        <v>33.33</v>
+        <v>25</v>
       </c>
       <c r="U25" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V25" s="1" t="n">
-        <v>33.33</v>
+        <v>37.5</v>
       </c>
       <c r="W25" s="1" t="n">
-        <v>1.33</v>
+        <v>1.38</v>
       </c>
       <c r="X25" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Y25" s="1" t="n">
-        <v>0.83</v>
+        <v>0.88</v>
       </c>
       <c r="Z25" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AA25" s="1" t="n">
         <v>1</v>
@@ -3236,40 +3236,40 @@
         <v>-1</v>
       </c>
       <c r="AC25" s="1" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AD25" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE25" s="1" t="n">
-        <v>46.15</v>
+        <v>46.67</v>
       </c>
       <c r="AF25" s="1" t="n">
         <v>5</v>
       </c>
       <c r="AG25" s="1" t="n">
-        <v>38.46</v>
+        <v>33.33</v>
       </c>
       <c r="AH25" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI25" s="1" t="n">
-        <v>15.38</v>
+        <v>20</v>
       </c>
       <c r="AJ25" s="1" t="n">
-        <v>1.77</v>
+        <v>1.73</v>
       </c>
       <c r="AK25" s="1" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AL25" s="1" t="n">
-        <v>1.31</v>
+        <v>1.27</v>
       </c>
       <c r="AM25" s="1" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AN25" s="1" t="n">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="AO25" s="1" t="n">
         <v>5</v>
@@ -3287,121 +3287,121 @@
         </is>
       </c>
       <c r="C26" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E26" s="1" t="n">
-        <v>66.67</v>
+        <v>57.14</v>
       </c>
       <c r="F26" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>16.67</v>
+        <v>28.57</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>16.67</v>
+        <v>14.29</v>
       </c>
       <c r="J26" s="1" t="n">
-        <v>2.17</v>
+        <v>2</v>
       </c>
       <c r="K26" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L26" s="1" t="n">
-        <v>2</v>
+        <v>1.86</v>
       </c>
       <c r="M26" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>0.67</v>
+        <v>0.71</v>
       </c>
       <c r="O26" s="1" t="n">
         <v>8</v>
       </c>
       <c r="P26" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q26" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R26" s="1" t="n">
-        <v>14.29</v>
+        <v>25</v>
       </c>
       <c r="S26" s="1" t="n">
         <v>2</v>
       </c>
       <c r="T26" s="1" t="n">
-        <v>28.57</v>
+        <v>25</v>
       </c>
       <c r="U26" s="1" t="n">
         <v>4</v>
       </c>
       <c r="V26" s="1" t="n">
-        <v>57.14</v>
+        <v>50</v>
       </c>
       <c r="W26" s="1" t="n">
-        <v>0.71</v>
+        <v>1</v>
       </c>
       <c r="X26" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y26" s="1" t="n">
-        <v>0.43</v>
+        <v>0.5</v>
       </c>
       <c r="Z26" s="1" t="n">
         <v>6</v>
       </c>
       <c r="AA26" s="1" t="n">
-        <v>0.86</v>
+        <v>0.75</v>
       </c>
       <c r="AB26" s="1" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="AC26" s="1" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AD26" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AE26" s="1" t="n">
-        <v>38.46</v>
+        <v>40</v>
       </c>
       <c r="AF26" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG26" s="1" t="n">
-        <v>23.08</v>
+        <v>26.67</v>
       </c>
       <c r="AH26" s="1" t="n">
         <v>5</v>
       </c>
       <c r="AI26" s="1" t="n">
-        <v>38.46</v>
+        <v>33.33</v>
       </c>
       <c r="AJ26" s="1" t="n">
-        <v>1.38</v>
+        <v>1.47</v>
       </c>
       <c r="AK26" s="1" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AL26" s="1" t="n">
-        <v>1.15</v>
+        <v>1.13</v>
       </c>
       <c r="AM26" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AN26" s="1" t="n">
-        <v>0.77</v>
+        <v>0.73</v>
       </c>
       <c r="AO26" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
@@ -3416,19 +3416,19 @@
         </is>
       </c>
       <c r="C27" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D27" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D27" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="E27" s="1" t="n">
-        <v>83.33</v>
+        <v>85.70999999999999</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>16.67</v>
+        <v>14.29</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>0</v>
@@ -3437,97 +3437,97 @@
         <v>0</v>
       </c>
       <c r="J27" s="1" t="n">
-        <v>2.67</v>
+        <v>2.71</v>
       </c>
       <c r="K27" s="1" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L27" s="1" t="n">
         <v>2</v>
       </c>
       <c r="M27" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N27" s="1" t="n">
-        <v>0.83</v>
+        <v>0.86</v>
       </c>
       <c r="O27" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="P27" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q27" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="R27" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="S27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="V27" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="W27" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="X27" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="P27" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="Q27" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="R27" s="1" t="n">
-        <v>57.14</v>
-      </c>
-      <c r="S27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U27" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="V27" s="1" t="n">
-        <v>42.86</v>
-      </c>
-      <c r="W27" s="1" t="n">
-        <v>1.71</v>
-      </c>
-      <c r="X27" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="Y27" s="1" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="Z27" s="1" t="n">
-        <v>6</v>
-      </c>
       <c r="AA27" s="1" t="n">
-        <v>0.86</v>
+        <v>0.88</v>
       </c>
       <c r="AB27" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC27" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="AD27" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE27" s="1" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="AF27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG27" s="1" t="n">
+        <v>6.67</v>
+      </c>
+      <c r="AH27" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI27" s="1" t="n">
+        <v>26.67</v>
+      </c>
+      <c r="AJ27" s="1" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="AK27" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL27" s="1" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="AM27" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="AD27" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="AE27" s="1" t="n">
-        <v>69.23</v>
-      </c>
-      <c r="AF27" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG27" s="1" t="n">
-        <v>7.69</v>
-      </c>
-      <c r="AH27" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AI27" s="1" t="n">
-        <v>23.08</v>
-      </c>
-      <c r="AJ27" s="1" t="n">
-        <v>2.15</v>
-      </c>
-      <c r="AK27" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="AL27" s="1" t="n">
-        <v>1.54</v>
-      </c>
-      <c r="AM27" s="1" t="n">
-        <v>11</v>
-      </c>
       <c r="AN27" s="1" t="n">
-        <v>0.85</v>
+        <v>0.87</v>
       </c>
       <c r="AO27" s="1" t="n">
         <v>9</v>
@@ -3584,13 +3584,13 @@
         <v>3</v>
       </c>
       <c r="P28" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q28" s="1" t="n">
         <v>5</v>
       </c>
       <c r="R28" s="1" t="n">
-        <v>83.33</v>
+        <v>71.43000000000001</v>
       </c>
       <c r="S28" s="1" t="n">
         <v>0</v>
@@ -3599,37 +3599,37 @@
         <v>0</v>
       </c>
       <c r="U28" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V28" s="1" t="n">
-        <v>16.67</v>
+        <v>28.57</v>
       </c>
       <c r="W28" s="1" t="n">
-        <v>2.5</v>
+        <v>2.14</v>
       </c>
       <c r="X28" s="1" t="n">
         <v>8</v>
       </c>
       <c r="Y28" s="1" t="n">
-        <v>1.33</v>
+        <v>1.14</v>
       </c>
       <c r="Z28" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA28" s="1" t="n">
-        <v>0.5</v>
+        <v>0.57</v>
       </c>
       <c r="AB28" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC28" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AD28" s="1" t="n">
         <v>9</v>
       </c>
       <c r="AE28" s="1" t="n">
-        <v>69.23</v>
+        <v>64.29000000000001</v>
       </c>
       <c r="AF28" s="1" t="n">
         <v>0</v>
@@ -3638,28 +3638,28 @@
         <v>0</v>
       </c>
       <c r="AH28" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI28" s="1" t="n">
-        <v>30.77</v>
+        <v>35.71</v>
       </c>
       <c r="AJ28" s="1" t="n">
-        <v>2.08</v>
+        <v>1.93</v>
       </c>
       <c r="AK28" s="1" t="n">
         <v>15</v>
       </c>
       <c r="AL28" s="1" t="n">
-        <v>1.15</v>
+        <v>1.07</v>
       </c>
       <c r="AM28" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="AN28" s="1" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="AO28" s="1" t="n">
         <v>7</v>
-      </c>
-      <c r="AN28" s="1" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="AO28" s="1" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="29">
@@ -3764,121 +3764,121 @@
         </is>
       </c>
       <c r="C31" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E31" s="1" t="n">
-        <v>71.43000000000001</v>
+        <v>75</v>
       </c>
       <c r="F31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="J31" s="1" t="n">
-        <v>2.29</v>
+        <v>2.38</v>
       </c>
       <c r="K31" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L31" s="1" t="n">
-        <v>2.14</v>
+        <v>2</v>
       </c>
       <c r="M31" s="1" t="n">
         <v>6</v>
       </c>
       <c r="N31" s="1" t="n">
-        <v>0.86</v>
+        <v>0.75</v>
       </c>
       <c r="O31" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P31" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q31" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R31" s="1" t="n">
-        <v>42.86</v>
+        <v>50</v>
       </c>
       <c r="S31" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T31" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="U31" s="1" t="n">
         <v>3</v>
       </c>
       <c r="V31" s="1" t="n">
-        <v>42.86</v>
+        <v>37.5</v>
       </c>
       <c r="W31" s="1" t="n">
-        <v>1.43</v>
+        <v>1.63</v>
       </c>
       <c r="X31" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="Y31" s="1" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="Z31" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA31" s="1" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="AB31" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC31" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AD31" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE31" s="1" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="AF31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG31" s="1" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="AH31" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI31" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK31" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AL31" s="1" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="AM31" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AN31" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="AO31" s="1" t="n">
         <v>13</v>
-      </c>
-      <c r="Y31" s="1" t="n">
-        <v>1.86</v>
-      </c>
-      <c r="Z31" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="AA31" s="1" t="n">
-        <v>1.57</v>
-      </c>
-      <c r="AB31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC31" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="AD31" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="AE31" s="1" t="n">
-        <v>57.14</v>
-      </c>
-      <c r="AF31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AG31" s="1" t="n">
-        <v>14.29</v>
-      </c>
-      <c r="AH31" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AI31" s="1" t="n">
-        <v>28.57</v>
-      </c>
-      <c r="AJ31" s="1" t="n">
-        <v>1.86</v>
-      </c>
-      <c r="AK31" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="AL31" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM31" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="AN31" s="1" t="n">
-        <v>1.21</v>
-      </c>
-      <c r="AO31" s="1" t="n">
-        <v>11</v>
       </c>
     </row>
     <row r="32">
@@ -3893,13 +3893,13 @@
         </is>
       </c>
       <c r="C32" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E32" s="1" t="n">
-        <v>71.43000000000001</v>
+        <v>75</v>
       </c>
       <c r="F32" s="1" t="n">
         <v>0</v>
@@ -3911,70 +3911,70 @@
         <v>2</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>28.57</v>
+        <v>25</v>
       </c>
       <c r="J32" s="1" t="n">
-        <v>2.14</v>
+        <v>2.25</v>
       </c>
       <c r="K32" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L32" s="1" t="n">
-        <v>1.86</v>
+        <v>1.75</v>
       </c>
       <c r="M32" s="1" t="n">
         <v>6</v>
       </c>
       <c r="N32" s="1" t="n">
-        <v>0.86</v>
+        <v>0.75</v>
       </c>
       <c r="O32" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P32" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q32" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R32" s="1" t="n">
-        <v>28.57</v>
+        <v>25</v>
       </c>
       <c r="S32" s="1" t="n">
         <v>3</v>
       </c>
       <c r="T32" s="1" t="n">
-        <v>42.86</v>
+        <v>37.5</v>
       </c>
       <c r="U32" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V32" s="1" t="n">
-        <v>28.57</v>
+        <v>37.5</v>
       </c>
       <c r="W32" s="1" t="n">
-        <v>1.29</v>
+        <v>1.13</v>
       </c>
       <c r="X32" s="1" t="n">
         <v>8</v>
       </c>
       <c r="Y32" s="1" t="n">
-        <v>1.14</v>
+        <v>1</v>
       </c>
       <c r="Z32" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA32" s="1" t="n">
-        <v>1.29</v>
+        <v>1.25</v>
       </c>
       <c r="AB32" s="1" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AC32" s="1" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AD32" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AE32" s="1" t="n">
         <v>50</v>
@@ -3983,28 +3983,28 @@
         <v>3</v>
       </c>
       <c r="AG32" s="1" t="n">
-        <v>21.43</v>
+        <v>18.75</v>
       </c>
       <c r="AH32" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI32" s="1" t="n">
-        <v>28.57</v>
+        <v>31.25</v>
       </c>
       <c r="AJ32" s="1" t="n">
-        <v>1.71</v>
+        <v>1.69</v>
       </c>
       <c r="AK32" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AL32" s="1" t="n">
-        <v>1.5</v>
+        <v>1.38</v>
       </c>
       <c r="AM32" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AN32" s="1" t="n">
-        <v>1.07</v>
+        <v>1</v>
       </c>
       <c r="AO32" s="1" t="n">
         <v>6</v>
@@ -4022,19 +4022,19 @@
         </is>
       </c>
       <c r="C33" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>71.43000000000001</v>
+        <v>75</v>
       </c>
       <c r="F33" s="1" t="n">
         <v>2</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>28.57</v>
+        <v>25</v>
       </c>
       <c r="H33" s="1" t="n">
         <v>0</v>
@@ -4043,31 +4043,31 @@
         <v>0</v>
       </c>
       <c r="J33" s="1" t="n">
-        <v>2.43</v>
+        <v>2.5</v>
       </c>
       <c r="K33" s="1" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L33" s="1" t="n">
-        <v>3.29</v>
+        <v>3</v>
       </c>
       <c r="M33" s="1" t="n">
         <v>8</v>
       </c>
       <c r="N33" s="1" t="n">
-        <v>1.14</v>
+        <v>1</v>
       </c>
       <c r="O33" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P33" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q33" s="1" t="n">
         <v>4</v>
       </c>
       <c r="R33" s="1" t="n">
-        <v>57.14</v>
+        <v>50</v>
       </c>
       <c r="S33" s="1" t="n">
         <v>0</v>
@@ -4076,64 +4076,64 @@
         <v>0</v>
       </c>
       <c r="U33" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V33" s="1" t="n">
-        <v>42.86</v>
+        <v>50</v>
       </c>
       <c r="W33" s="1" t="n">
-        <v>1.71</v>
+        <v>1.5</v>
       </c>
       <c r="X33" s="1" t="n">
         <v>12</v>
       </c>
       <c r="Y33" s="1" t="n">
-        <v>1.71</v>
+        <v>1.5</v>
       </c>
       <c r="Z33" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AA33" s="1" t="n">
-        <v>0.86</v>
+        <v>0.88</v>
       </c>
       <c r="AB33" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AC33" s="1" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AD33" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AE33" s="1" t="n">
-        <v>64.29000000000001</v>
+        <v>62.5</v>
       </c>
       <c r="AF33" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AG33" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="AH33" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AI33" s="1" t="n">
-        <v>21.43</v>
+        <v>25</v>
       </c>
       <c r="AJ33" s="1" t="n">
-        <v>2.07</v>
+        <v>2</v>
       </c>
       <c r="AK33" s="1" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AL33" s="1" t="n">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="AM33" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AN33" s="1" t="n">
-        <v>1</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="AO33" s="1" t="n">
         <v>21</v>
@@ -4190,82 +4190,82 @@
         <v>4</v>
       </c>
       <c r="P34" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q34" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R34" s="1" t="n">
-        <v>33.33</v>
+        <v>25</v>
       </c>
       <c r="S34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T34" s="1" t="n">
-        <v>16.67</v>
+        <v>12.5</v>
       </c>
       <c r="U34" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V34" s="1" t="n">
-        <v>50</v>
+        <v>62.5</v>
       </c>
       <c r="W34" s="1" t="n">
-        <v>1.17</v>
+        <v>0.88</v>
       </c>
       <c r="X34" s="1" t="n">
         <v>10</v>
       </c>
       <c r="Y34" s="1" t="n">
-        <v>1.67</v>
+        <v>1.25</v>
       </c>
       <c r="Z34" s="1" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AA34" s="1" t="n">
-        <v>2.17</v>
+        <v>1.88</v>
       </c>
       <c r="AB34" s="1" t="n">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="AC34" s="1" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AD34" s="1" t="n">
         <v>7</v>
       </c>
       <c r="AE34" s="1" t="n">
-        <v>50</v>
+        <v>43.75</v>
       </c>
       <c r="AF34" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AG34" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="AH34" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AI34" s="1" t="n">
-        <v>35.71</v>
+        <v>43.75</v>
       </c>
       <c r="AJ34" s="1" t="n">
-        <v>1.64</v>
+        <v>1.44</v>
       </c>
       <c r="AK34" s="1" t="n">
         <v>26</v>
       </c>
       <c r="AL34" s="1" t="n">
-        <v>1.86</v>
+        <v>1.62</v>
       </c>
       <c r="AM34" s="1" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AN34" s="1" t="n">
-        <v>1.79</v>
+        <v>1.69</v>
       </c>
       <c r="AO34" s="1" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="35">
@@ -4280,121 +4280,121 @@
         </is>
       </c>
       <c r="C35" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D35" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>57.14</v>
+        <v>50</v>
       </c>
       <c r="F35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G35" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>28.57</v>
+        <v>37.5</v>
       </c>
       <c r="J35" s="1" t="n">
-        <v>1.86</v>
+        <v>1.63</v>
       </c>
       <c r="K35" s="1" t="n">
         <v>11</v>
       </c>
       <c r="L35" s="1" t="n">
-        <v>1.57</v>
+        <v>1.38</v>
       </c>
       <c r="M35" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N35" s="1" t="n">
-        <v>1.43</v>
+        <v>1.38</v>
       </c>
       <c r="O35" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P35" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R35" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="S35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T35" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="U35" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="V35" s="1" t="n">
-        <v>71.43000000000001</v>
+        <v>75</v>
       </c>
       <c r="W35" s="1" t="n">
-        <v>0.57</v>
+        <v>0.5</v>
       </c>
       <c r="X35" s="1" t="n">
         <v>8</v>
       </c>
       <c r="Y35" s="1" t="n">
-        <v>1.14</v>
+        <v>1</v>
       </c>
       <c r="Z35" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA35" s="1" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="AB35" s="1" t="n">
+        <v>-10</v>
+      </c>
+      <c r="AC35" s="1" t="n">
         <v>16</v>
-      </c>
-      <c r="AA35" s="1" t="n">
-        <v>2.29</v>
-      </c>
-      <c r="AB35" s="1" t="n">
-        <v>-8</v>
-      </c>
-      <c r="AC35" s="1" t="n">
-        <v>14</v>
       </c>
       <c r="AD35" s="1" t="n">
         <v>5</v>
       </c>
       <c r="AE35" s="1" t="n">
-        <v>35.71</v>
+        <v>31.25</v>
       </c>
       <c r="AF35" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AG35" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="AH35" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AI35" s="1" t="n">
-        <v>50</v>
+        <v>56.25</v>
       </c>
       <c r="AJ35" s="1" t="n">
-        <v>1.21</v>
+        <v>1.06</v>
       </c>
       <c r="AK35" s="1" t="n">
         <v>19</v>
       </c>
       <c r="AL35" s="1" t="n">
-        <v>1.36</v>
+        <v>1.19</v>
       </c>
       <c r="AM35" s="1" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="AN35" s="1" t="n">
-        <v>1.86</v>
+        <v>1.81</v>
       </c>
       <c r="AO35" s="1" t="n">
-        <v>-7</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="36">
@@ -4409,19 +4409,19 @@
         </is>
       </c>
       <c r="C36" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D36" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D36" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="E36" s="1" t="n">
-        <v>83.33</v>
+        <v>85.70999999999999</v>
       </c>
       <c r="F36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>16.67</v>
+        <v>14.29</v>
       </c>
       <c r="H36" s="1" t="n">
         <v>0</v>
@@ -4430,100 +4430,100 @@
         <v>0</v>
       </c>
       <c r="J36" s="1" t="n">
-        <v>2.67</v>
+        <v>2.71</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="L36" s="1" t="n">
-        <v>2</v>
+        <v>2.43</v>
       </c>
       <c r="M36" s="1" t="n">
         <v>3</v>
       </c>
       <c r="N36" s="1" t="n">
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="O36" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="P36" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="P36" s="1" t="n">
-        <v>8</v>
-      </c>
       <c r="Q36" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R36" s="1" t="n">
-        <v>50</v>
+        <v>55.56</v>
       </c>
       <c r="S36" s="1" t="n">
         <v>2</v>
       </c>
       <c r="T36" s="1" t="n">
-        <v>25</v>
+        <v>22.22</v>
       </c>
       <c r="U36" s="1" t="n">
         <v>2</v>
       </c>
       <c r="V36" s="1" t="n">
-        <v>25</v>
+        <v>22.22</v>
       </c>
       <c r="W36" s="1" t="n">
-        <v>1.75</v>
+        <v>1.89</v>
       </c>
       <c r="X36" s="1" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="Y36" s="1" t="n">
-        <v>1.88</v>
+        <v>2</v>
       </c>
       <c r="Z36" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AA36" s="1" t="n">
-        <v>1.12</v>
+        <v>1.22</v>
       </c>
       <c r="AB36" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC36" s="1" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AD36" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AE36" s="1" t="n">
-        <v>64.29000000000001</v>
+        <v>68.75</v>
       </c>
       <c r="AF36" s="1" t="n">
         <v>3</v>
       </c>
       <c r="AG36" s="1" t="n">
-        <v>21.43</v>
+        <v>18.75</v>
       </c>
       <c r="AH36" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AI36" s="1" t="n">
-        <v>14.29</v>
+        <v>12.5</v>
       </c>
       <c r="AJ36" s="1" t="n">
-        <v>2.14</v>
+        <v>2.25</v>
       </c>
       <c r="AK36" s="1" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="AL36" s="1" t="n">
-        <v>1.93</v>
+        <v>2.19</v>
       </c>
       <c r="AM36" s="1" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AN36" s="1" t="n">
-        <v>0.86</v>
+        <v>0.88</v>
       </c>
       <c r="AO36" s="1" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>